<commit_message>
Updated collection data in Mayibuye Events collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/MAYIBUYE EVENTS COLLECTION.xlsx
+++ b/Photographic Archive/MAYIBUYE EVENTS COLLECTION.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$756</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -7333,9 +7333,9 @@
   </sheetPr>
   <dimension ref="A1:AA756"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7348,7 +7348,7 @@
     <col min="8" max="8" width="39.44140625" customWidth="1"/>
     <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="12" max="15" width="12.6640625" customWidth="1"/>
+    <col min="12" max="15" width="12.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>